<commit_message>
adddd notes from Sarah, and modifed benchmark results and wrote some of the report
</commit_message>
<xml_diff>
--- a/Busca Report/Benchmark results (hugo machine).xlsx
+++ b/Busca Report/Benchmark results (hugo machine).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Google Drive\Education\ITU\1st Semester\Introductory Programming\Busca\ip18groupR\Busca Report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ieva.kangsepa\IdeaProjects\REPORT\Busca Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D7C48B-2DE0-4DA4-BBCB-D32CC6AA62D2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0BD3A05-3EC3-4998-8C28-858A4F82828C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9648" xr2:uid="{28DDE827-F72A-4FC2-994A-DC90B1FA214D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="23">
   <si>
     <t>Index</t>
   </si>
@@ -64,6 +64,36 @@
   </si>
   <si>
     <t>± Error of uncertainty</t>
+  </si>
+  <si>
+    <t>New Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ± 277.782</t>
+  </si>
+  <si>
+    <t>± 64.279</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ± 22.917</t>
+  </si>
+  <si>
+    <t>± 459629.261</t>
+  </si>
+  <si>
+    <t>± 74.249</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ± 37.409</t>
+  </si>
+  <si>
+    <t>± 4376354.480</t>
+  </si>
+  <si>
+    <t>± 415.305</t>
+  </si>
+  <si>
+    <t>± 390.336</t>
   </si>
 </sst>
 </file>
@@ -416,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAAFAD8E-C445-43BD-8978-1BED714D60E6}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -705,6 +735,203 @@
         <v>11</v>
       </c>
     </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <v>30176.992999999999</v>
+      </c>
+      <c r="C18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19">
+        <v>27451.02</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20">
+        <v>233498546.57100001</v>
+      </c>
+      <c r="C20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25">
+        <v>3622.5819999999999</v>
+      </c>
+      <c r="C25" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26">
+        <v>1883.7760000000001</v>
+      </c>
+      <c r="C26" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27">
+        <v>8819338.5920000002</v>
+      </c>
+      <c r="C27" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31">
+        <v>1591.3109999999999</v>
+      </c>
+      <c r="C31" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32">
+        <v>1052.067</v>
+      </c>
+      <c r="C32" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33">
+        <v>18944.883999999998</v>
+      </c>
+      <c r="C33" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>